<commit_message>
get the relation between num_image and ratio
</commit_message>
<xml_diff>
--- a/group3.xlsx
+++ b/group3.xlsx
@@ -35,6 +35,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -116,7 +117,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
@@ -228,29 +229,77 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>64.83</v>
+        <v>30</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>63.8</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>62.57</v>
+        <v>45.79</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>55.78</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>64.83</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>63.8</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>62.57</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>70.51</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>75.74</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>79.72</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>83.1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B15" s="0" t="n">
         <v>87.82</v>
       </c>
-      <c r="C9" s="0" t="n">
-        <v>85.45</v>
-      </c>
-      <c r="D9" s="0" t="n">
+      <c r="C15" s="0" t="n">
+        <v>85.47</v>
+      </c>
+      <c r="D15" s="0" t="n">
         <v>82.56</v>
       </c>
     </row>

</xml_diff>